<commit_message>
Agregadas nuevas actividades internas en el CI5
</commit_message>
<xml_diff>
--- a/Planificación del proyecto/CI5 Equipo 01.xlsx
+++ b/Planificación del proyecto/CI5 Equipo 01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeDicenTecno\Desktop\proyect\Ecommerce-Sports\Planificación del proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="300">
   <si>
     <t>Nro Hito</t>
   </si>
@@ -914,7 +914,16 @@
     <t>1:30 hs.</t>
   </si>
   <si>
-    <t>SEMANA 5: No hay NUEVAS actividades recpecto a CC2</t>
+    <t>Ofertas</t>
+  </si>
+  <si>
+    <t>Implementar política de Ofertas</t>
+  </si>
+  <si>
+    <t>Establecer dependencias y listar ofertas</t>
+  </si>
+  <si>
+    <t>07/010/2020</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1011,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1024,12 +1033,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1393,29 +1396,23 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1433,7 +1430,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1656,8 +1659,8 @@
   </sheetPr>
   <dimension ref="A1:AA112"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53:N53"/>
+    <sheetView topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5780,91 +5783,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="82"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="74" t="s">
+      <c r="O1" s="82"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="75"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="82"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="74" t="s">
+      <c r="U1" s="82"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="82"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="74" t="s">
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="74" t="s">
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="76"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="83"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="78"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -5947,20 +5950,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -35986,16 +35989,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
@@ -36004,6 +35997,16 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -36028,91 +36031,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="75"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="82"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="74" t="s">
+      <c r="O1" s="82"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="75"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="82"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="74" t="s">
+      <c r="U1" s="82"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="82"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="74" t="s">
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="82"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="74" t="s">
+      <c r="AG1" s="82"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="76"/>
+      <c r="AJ1" s="82"/>
+      <c r="AK1" s="83"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="78"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -36195,20 +36198,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -38686,12 +38689,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -38704,6 +38701,12 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38727,79 +38730,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="74" t="s">
+      <c r="O1" s="90"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="85"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="74" t="s">
+      <c r="U1" s="90"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="90"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="74" t="s">
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="74" t="s">
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="86"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="91"/>
       <c r="AL1" s="39"/>
       <c r="AM1" s="66"/>
       <c r="AN1" s="66"/>
@@ -38810,16 +38813,16 @@
       <c r="AS1" s="53"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A2" s="87"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -38910,20 +38913,20 @@
       <c r="AS2" s="53"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A3" s="88"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -43913,12 +43916,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -43931,6 +43928,12 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43956,91 +43959,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="74" t="s">
+      <c r="O1" s="90"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="85"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="74" t="s">
+      <c r="U1" s="90"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="90"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="74" t="s">
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="74" t="s">
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="86"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="91"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="87"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -44123,20 +44126,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="88"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -48922,6 +48925,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -48934,12 +48943,6 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48949,8 +48952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="S43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI62" sqref="AI62:AK64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -48968,91 +48971,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="H1" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="80" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="85"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="74" t="s">
+      <c r="O1" s="90"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="80" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="85"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="74" t="s">
+      <c r="U1" s="90"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="80" t="s">
+      <c r="X1" s="90"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="74" t="s">
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="80" t="s">
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="86"/>
-      <c r="AI1" s="74" t="s">
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="86"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="91"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A2" s="87"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
       <c r="K2" s="3">
         <v>44081</v>
       </c>
@@ -49135,20 +49138,20 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A3" s="88"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
       <c r="K3" s="9" t="s">
         <v>36</v>
       </c>
@@ -52819,90 +52822,120 @@
       <c r="AK62" s="45"/>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
+      <c r="A63" s="39">
+        <v>61</v>
+      </c>
       <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
+      <c r="C63" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="D63" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E63" s="39" t="s">
+        <v>111</v>
+      </c>
       <c r="F63" s="39"/>
-      <c r="G63" s="71"/>
-      <c r="H63" s="71"/>
-      <c r="I63" s="71"/>
+      <c r="G63" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="H63" s="70">
+        <v>44109</v>
+      </c>
+      <c r="I63" s="70">
+        <v>44122</v>
+      </c>
       <c r="J63" s="39"/>
-      <c r="K63" s="71"/>
-      <c r="L63" s="71"/>
-      <c r="M63" s="71"/>
-      <c r="N63" s="71"/>
-      <c r="O63" s="71"/>
-      <c r="P63" s="71"/>
-      <c r="Q63" s="71"/>
-      <c r="R63" s="71"/>
-      <c r="S63" s="71"/>
-      <c r="T63" s="71"/>
-      <c r="U63" s="71"/>
-      <c r="V63" s="71"/>
-      <c r="W63" s="71"/>
-      <c r="X63" s="71"/>
-      <c r="Y63" s="71"/>
-      <c r="Z63" s="71"/>
-      <c r="AA63" s="71"/>
-      <c r="AB63" s="71"/>
-      <c r="AC63" s="71"/>
-      <c r="AD63" s="71"/>
-      <c r="AE63" s="71"/>
-      <c r="AF63" s="71"/>
-      <c r="AG63" s="71"/>
-      <c r="AH63" s="71"/>
-      <c r="AI63" s="71"/>
-      <c r="AJ63" s="71"/>
-      <c r="AK63" s="71"/>
+      <c r="K63" s="45"/>
+      <c r="L63" s="45"/>
+      <c r="M63" s="45"/>
+      <c r="N63" s="69"/>
+      <c r="O63" s="69"/>
+      <c r="P63" s="69"/>
+      <c r="Q63" s="45"/>
+      <c r="R63" s="45"/>
+      <c r="S63" s="45"/>
+      <c r="T63" s="69"/>
+      <c r="U63" s="69"/>
+      <c r="V63" s="69"/>
+      <c r="W63" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="X63" s="45"/>
+      <c r="Y63" s="45"/>
+      <c r="Z63" s="69"/>
+      <c r="AA63" s="69"/>
+      <c r="AB63" s="69"/>
+      <c r="AC63" s="45"/>
+      <c r="AD63" s="45"/>
+      <c r="AE63" s="45"/>
+      <c r="AF63" s="69"/>
+      <c r="AG63" s="69"/>
+      <c r="AH63" s="69"/>
+      <c r="AI63" s="45"/>
+      <c r="AJ63" s="45"/>
+      <c r="AK63" s="45"/>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
+      <c r="A64" s="39">
+        <v>62</v>
+      </c>
       <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
+      <c r="C64" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="D64" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>152</v>
+      </c>
       <c r="F64" s="39"/>
-      <c r="G64" s="71"/>
-      <c r="H64" s="71"/>
-      <c r="I64" s="71"/>
+      <c r="G64" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H64" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="I64" s="70">
+        <v>44122</v>
+      </c>
       <c r="J64" s="39"/>
-      <c r="K64" s="71"/>
-      <c r="L64" s="71"/>
-      <c r="M64" s="71"/>
-      <c r="N64" s="71"/>
-      <c r="O64" s="71"/>
-      <c r="P64" s="71"/>
-      <c r="Q64" s="71"/>
-      <c r="R64" s="71"/>
-      <c r="S64" s="71"/>
-      <c r="T64" s="71"/>
-      <c r="U64" s="71"/>
-      <c r="V64" s="71"/>
-      <c r="W64" s="71"/>
-      <c r="X64" s="71"/>
-      <c r="Y64" s="71"/>
-      <c r="Z64" s="71"/>
-      <c r="AA64" s="71"/>
-      <c r="AB64" s="71"/>
-      <c r="AC64" s="71"/>
-      <c r="AD64" s="71"/>
-      <c r="AE64" s="71"/>
-      <c r="AF64" s="71"/>
-      <c r="AG64" s="71"/>
-      <c r="AH64" s="71"/>
-      <c r="AI64" s="71"/>
-      <c r="AJ64" s="71"/>
-      <c r="AK64" s="71"/>
+      <c r="K64" s="45"/>
+      <c r="L64" s="45"/>
+      <c r="M64" s="45"/>
+      <c r="N64" s="69"/>
+      <c r="O64" s="69"/>
+      <c r="P64" s="69"/>
+      <c r="Q64" s="45"/>
+      <c r="R64" s="45"/>
+      <c r="S64" s="45"/>
+      <c r="T64" s="69"/>
+      <c r="U64" s="69"/>
+      <c r="V64" s="69"/>
+      <c r="W64" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="X64" s="45"/>
+      <c r="Y64" s="45"/>
+      <c r="Z64" s="69"/>
+      <c r="AA64" s="69"/>
+      <c r="AB64" s="69"/>
+      <c r="AC64" s="45"/>
+      <c r="AD64" s="45"/>
+      <c r="AE64" s="45"/>
+      <c r="AF64" s="69"/>
+      <c r="AG64" s="69"/>
+      <c r="AH64" s="69"/>
+      <c r="AI64" s="45"/>
+      <c r="AJ64" s="45"/>
+      <c r="AK64" s="45"/>
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A65" s="71"/>
       <c r="B65" s="71"/>
       <c r="C65" s="71"/>
-      <c r="D65" s="92" t="s">
-        <v>296</v>
-      </c>
+      <c r="D65" s="92"/>
       <c r="E65" s="71"/>
       <c r="F65" s="71"/>
       <c r="G65" s="71"/>
@@ -52939,12 +52972,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -52957,6 +52984,12 @@
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>